<commit_message>
fixed the days table and the end day
</commit_message>
<xml_diff>
--- a/SourceDocuments/InPut_Excel/Watch_List.xlsx
+++ b/SourceDocuments/InPut_Excel/Watch_List.xlsx
@@ -16,30 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>MEGL</t>
-  </si>
-  <si>
-    <t>AGBA</t>
-  </si>
-  <si>
-    <t>SIEB</t>
-  </si>
-  <si>
-    <t>TPST</t>
-  </si>
-  <si>
-    <t>GSUN</t>
-  </si>
-  <si>
-    <t>HUDI</t>
-  </si>
-  <si>
-    <t>WLGS</t>
-  </si>
-  <si>
-    <t>TCJH</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -47,6 +23,30 @@
   </si>
   <si>
     <t>mmm</t>
+  </si>
+  <si>
+    <t>CRKN</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>GOOGL</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>LCID</t>
+  </si>
+  <si>
+    <t>NVDA</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,50 +409,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>45119</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>45109</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>45119</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>45041</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>45119</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,31 +460,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>45142</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>45142</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>45142</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1">
-        <v>45142</v>
+        <v>45156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>